<commit_message>
added a login component, not functional yet
</commit_message>
<xml_diff>
--- a/databaseSql/database tables.xlsx
+++ b/databaseSql/database tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\Documents\uniwersytet\rok_3\3000\databaseSql\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\Documents\uniwersytet\rok_3\3000\repository\Comp-3000-Patryk-Rog\databaseSql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2A9A67-AEFE-46BB-B2A7-DB73973EA2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD75DA3B-0D72-478A-BB32-0C45A936F643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{430FD31B-1F62-40E9-BC85-188A60A506D0}"/>
+    <workbookView xWindow="18165" yWindow="0" windowWidth="10740" windowHeight="15585" xr2:uid="{430FD31B-1F62-40E9-BC85-188A60A506D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>TABLES</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t>comment_content</t>
+  </si>
+  <si>
+    <t>RESTAURANT USERS</t>
+  </si>
+  <si>
+    <t>account_type</t>
   </si>
 </sst>
 </file>
@@ -534,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C97FB63F-CA3B-4245-8C77-2A286852E3C0}">
-  <dimension ref="B2:K31"/>
+  <dimension ref="B2:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,7 +681,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>6</v>
       </c>
@@ -685,8 +691,11 @@
       <c r="G25" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>31</v>
       </c>
@@ -696,8 +705,11 @@
       <c r="G26" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>26</v>
       </c>
@@ -707,8 +719,11 @@
       <c r="G27" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>32</v>
       </c>
@@ -718,8 +733,11 @@
       <c r="G28" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>33</v>
       </c>
@@ -729,18 +747,32 @@
       <c r="G29" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>34</v>
       </c>
       <c r="G30" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
       <c r="G31" t="s">
         <v>41</v>
+      </c>
+      <c r="I31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edited sql for restaurant users table and created a procedure for user creation
</commit_message>
<xml_diff>
--- a/databaseSql/database tables.xlsx
+++ b/databaseSql/database tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\Documents\uniwersytet\rok_3\3000\repository\Comp-3000-Patryk-Rog\databaseSql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD75DA3B-0D72-478A-BB32-0C45A936F643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD758D1-9319-454A-B719-24F9A1508206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18165" yWindow="0" windowWidth="10740" windowHeight="15585" xr2:uid="{430FD31B-1F62-40E9-BC85-188A60A506D0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{430FD31B-1F62-40E9-BC85-188A60A506D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>TABLES</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>account_type</t>
+  </si>
+  <si>
+    <t>date_of_birth</t>
   </si>
 </sst>
 </file>
@@ -540,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C97FB63F-CA3B-4245-8C77-2A286852E3C0}">
-  <dimension ref="B2:K32"/>
+  <dimension ref="B2:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,6 +778,11 @@
         <v>15</v>
       </c>
     </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added 3 tables for table booking and opening times, added sample data
</commit_message>
<xml_diff>
--- a/databaseSql/database tables.xlsx
+++ b/databaseSql/database tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\Documents\uniwersytet\rok_3\3000\repository\Comp-3000-Patryk-Rog\databaseSql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD758D1-9319-454A-B719-24F9A1508206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B07E89-8341-4595-B21B-9D05D76F90CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{430FD31B-1F62-40E9-BC85-188A60A506D0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
   <si>
     <t>TABLES</t>
   </si>
@@ -171,6 +171,36 @@
   </si>
   <si>
     <t>date_of_birth</t>
+  </si>
+  <si>
+    <t>opening_time</t>
+  </si>
+  <si>
+    <t>closing_time</t>
+  </si>
+  <si>
+    <t>RESTAURANT OPEN TIMES</t>
+  </si>
+  <si>
+    <t>day_of_week</t>
+  </si>
+  <si>
+    <t>TABLE</t>
+  </si>
+  <si>
+    <t>table_id</t>
+  </si>
+  <si>
+    <t>seating</t>
+  </si>
+  <si>
+    <t>TABLE BOOKINGS</t>
+  </si>
+  <si>
+    <t>table_bookings_id</t>
+  </si>
+  <si>
+    <t>booking_length</t>
   </si>
 </sst>
 </file>
@@ -543,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C97FB63F-CA3B-4245-8C77-2A286852E3C0}">
-  <dimension ref="B2:K33"/>
+  <dimension ref="B2:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,15 +585,16 @@
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>1</v>
       </c>
@@ -579,8 +610,11 @@
       <c r="K3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>9</v>
       </c>
@@ -596,8 +630,11 @@
       <c r="K4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>10</v>
       </c>
@@ -613,8 +650,11 @@
       <c r="K5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>11</v>
       </c>
@@ -630,8 +670,11 @@
       <c r="K6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>12</v>
       </c>
@@ -648,7 +691,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>13</v>
       </c>
@@ -665,7 +708,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>14</v>
       </c>
@@ -679,12 +722,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>6</v>
       </c>
@@ -697,8 +740,14 @@
       <c r="I25" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>47</v>
+      </c>
+      <c r="M25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>31</v>
       </c>
@@ -711,8 +760,14 @@
       <c r="I26" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
+        <v>15</v>
+      </c>
+      <c r="M26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>26</v>
       </c>
@@ -725,8 +780,14 @@
       <c r="I27" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K27" t="s">
+        <v>48</v>
+      </c>
+      <c r="M27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>32</v>
       </c>
@@ -739,8 +800,14 @@
       <c r="I28" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>45</v>
+      </c>
+      <c r="M28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>33</v>
       </c>
@@ -753,8 +820,14 @@
       <c r="I29" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K29" t="s">
+        <v>46</v>
+      </c>
+      <c r="M29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>34</v>
       </c>
@@ -764,16 +837,22 @@
       <c r="I30" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="M30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="3:13" x14ac:dyDescent="0.25">
       <c r="G31" t="s">
         <v>41</v>
       </c>
       <c r="I31" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="M31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13" x14ac:dyDescent="0.25">
       <c r="I32" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
added restaurant creation endpoint, modified sql
</commit_message>
<xml_diff>
--- a/databaseSql/database tables.xlsx
+++ b/databaseSql/database tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\Documents\uniwersytet\rok_3\3000\repository\Comp-3000-Patryk-Rog\databaseSql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A415EB3D-D45D-44AB-85F0-1177C1C33C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC5C108-7AB2-4601-B724-7E724B04256C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{430FD31B-1F62-40E9-BC85-188A60A506D0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
   <si>
     <t>TABLES</t>
   </si>
@@ -89,9 +89,6 @@
     <t>restuarant_name</t>
   </si>
   <si>
-    <t>total_tables</t>
-  </si>
-  <si>
     <t>restuarnt_description</t>
   </si>
   <si>
@@ -201,6 +198,15 @@
   </si>
   <si>
     <t>booking_length</t>
+  </si>
+  <si>
+    <t>restaurant_location</t>
+  </si>
+  <si>
+    <t>STAFF RESTAURANTS</t>
+  </si>
+  <si>
+    <t>user_id (restaurant users)</t>
   </si>
 </sst>
 </file>
@@ -573,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C97FB63F-CA3B-4245-8C77-2A286852E3C0}">
-  <dimension ref="B2:M33"/>
+  <dimension ref="B2:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,14 +593,15 @@
     <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22" customWidth="1"/>
+    <col min="15" max="15" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>1</v>
       </c>
@@ -611,10 +618,13 @@
         <v>5</v>
       </c>
       <c r="M3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="O3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>9</v>
       </c>
@@ -622,19 +632,22 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="O4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>10</v>
       </c>
@@ -648,83 +661,89 @@
         <v>15</v>
       </c>
       <c r="K5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="O5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="G6" t="s">
         <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="O6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
         <v>24</v>
-      </c>
-      <c r="I9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="G10" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="25" spans="3:13" x14ac:dyDescent="0.25">
@@ -738,24 +757,24 @@
         <v>8</v>
       </c>
       <c r="I25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E26" t="s">
         <v>9</v>
       </c>
       <c r="G26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I26" t="s">
         <v>9</v>
@@ -764,15 +783,15 @@
         <v>15</v>
       </c>
       <c r="M26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G27" t="s">
         <v>9</v>
@@ -781,18 +800,18 @@
         <v>12</v>
       </c>
       <c r="K27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G28" t="s">
         <v>15</v>
@@ -801,38 +820,38 @@
         <v>14</v>
       </c>
       <c r="K28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I30" t="s">
         <v>10</v>
@@ -843,13 +862,13 @@
     </row>
     <row r="31" spans="3:13" x14ac:dyDescent="0.25">
       <c r="G31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I31" t="s">
         <v>11</v>
       </c>
       <c r="M31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="3:13" x14ac:dyDescent="0.25">
@@ -859,7 +878,7 @@
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added api endpoint for table creation, adjusted sql, created table creator component
</commit_message>
<xml_diff>
--- a/databaseSql/database tables.xlsx
+++ b/databaseSql/database tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\Documents\uniwersytet\rok_3\3000\repository\Comp-3000-Patryk-Rog\databaseSql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC5C108-7AB2-4601-B724-7E724B04256C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0630428-6BAA-46B0-BA27-B2A1902DC1FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{430FD31B-1F62-40E9-BC85-188A60A506D0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
   <si>
     <t>TABLES</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>user_id (restaurant users)</t>
+  </si>
+  <si>
+    <t>table_no</t>
   </si>
 </sst>
 </file>
@@ -582,7 +585,7 @@
   <dimension ref="B2:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,6 +712,9 @@
       <c r="K7" t="s">
         <v>32</v>
       </c>
+      <c r="M7" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C8" t="s">

</xml_diff>